<commit_message>
onlly get good camps
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -417,10 +417,10 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>3334</v>
+        <v>3003</v>
       </c>
       <c r="C2">
-        <v>5413</v>
+        <v>5257</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -428,10 +428,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>1730</v>
+        <v>1637</v>
       </c>
       <c r="C3">
-        <v>2259</v>
+        <v>2247</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -439,10 +439,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>1082</v>
+        <v>1030</v>
       </c>
       <c r="C4">
-        <v>2208</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -450,10 +450,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>522</v>
+        <v>336</v>
       </c>
       <c r="C5">
-        <v>946</v>
+        <v>932</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -461,10 +461,10 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.289</v>
+        <v>0.351</v>
       </c>
       <c r="C6">
-        <v>0.199</v>
+        <v>0.193</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -472,10 +472,10 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>2273196</v>
+        <v>2110705</v>
       </c>
       <c r="C7">
-        <v>3725198</v>
+        <v>3668754</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -483,10 +483,10 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.319</v>
+        <v>0.327</v>
       </c>
       <c r="C8">
-        <v>0.545</v>
+        <v>0.5570000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>